<commit_message>
remove extraneous sheet from titering
</commit_message>
<xml_diff>
--- a/experimental_validations/data/210125_mutvirus_titering_HAARVI.xlsx
+++ b/experimental_validations/data/210125_mutvirus_titering_HAARVI.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\VEP_DMS_Barcode\plate_reader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/fh/fast/bloom_j/computational_notebooks/kdusenbu/2021/SARS-CoV-2-RBD_MAP_HAARVI_sera/experimental_validations/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F27CCD7-E7E8-4560-9A27-3D75228D0AB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D06134-2464-7B48-AC1E-6B5B92CD16E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4485" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{7C440C55-AA6A-41B3-88C0-D7663FC47812}"/>
+    <workbookView xWindow="4480" yWindow="2980" windowWidth="21600" windowHeight="11380" xr2:uid="{7C440C55-AA6A-41B3-88C0-D7663FC47812}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plate5-2" sheetId="8" r:id="rId1"/>
-    <sheet name="Plate6" sheetId="7" r:id="rId2"/>
-    <sheet name="Plate5" sheetId="6" r:id="rId3"/>
-    <sheet name="Plate4" sheetId="5" r:id="rId4"/>
-    <sheet name="Plate3" sheetId="4" r:id="rId5"/>
-    <sheet name="Plate2" sheetId="3" r:id="rId6"/>
-    <sheet name="Plate1" sheetId="2" r:id="rId7"/>
+    <sheet name="Plate6" sheetId="7" r:id="rId1"/>
+    <sheet name="Plate5" sheetId="6" r:id="rId2"/>
+    <sheet name="Plate4" sheetId="5" r:id="rId3"/>
+    <sheet name="Plate3" sheetId="4" r:id="rId4"/>
+    <sheet name="Plate2" sheetId="3" r:id="rId5"/>
+    <sheet name="Plate1" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,100 +38,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Dusenbury Crawford, Katharine H</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{6AFAB3EC-BD3D-4CBD-879F-60750E7C9714}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Tecan.At.Common, 3.9.1.0
-Tecan.At.Common.DocumentManagement, 3.9.1.0
-Tecan.At.Common.DocumentManagement.Reader, 3.6.1.0
-Tecan.At.Common.MCS, 3.9.1.0
-Tecan.At.Common.Results, 3.9.1.0
-Tecan.At.Common.UI, 3.9.1.0
-Tecan.At.Communication.Common, 3.9.1.0
-Tecan.At.Communication.Port.IP, 3.9.1.0
-Tecan.At.Communication.Port.RS232, 3.9.1.0
-Tecan.At.Communication.Port.SIM.Common, 3.9.1.0
-Tecan.At.Communication.Port.USB, 3.9.1.0
-Tecan.At.Communication.Server, 3.9.1.0
-Tecan.At.Communication.SIM.AMR, 3.6.1.0
-Tecan.At.Communication.SIM.AMRPlus, 3.6.1.0
-Tecan.At.Communication.SIM.Connect, 3.9.1.0
-Tecan.At.Communication.SIM.GeniosUltra, 3.6.1.0
-Tecan.At.Communication.SIM.Safire3, 3.6.1.0
-Tecan.At.Communication.SIM.Safire3Pro, 3.6.1.0
-Tecan.At.Communication.SIM.SunriseMini, 3.6.1.0
-Tecan.At.Instrument.Common, 3.9.1.0
-Tecan.At.Instrument.Common.GCM, 3.9.1.0
-Tecan.At.Instrument.Common.Reader, 3.6.1.0
-Tecan.At.Instrument.Common.Stacker, 3.9.1.0
-Tecan.At.Instrument.Gas.GCM, 3.9.1.0
-Tecan.At.Instrument.GCM.Server, 3.9.1.0
-Tecan.At.Instrument.Reader.AMR, 3.6.1.0
-Tecan.At.Instrument.Reader.AMRPlus, 3.6.1.0
-Tecan.At.Instrument.Reader.GeniosUltra, 3.6.1.0
-Tecan.At.Instrument.Reader.Safire3, 3.6.1.0
-Tecan.At.Instrument.Reader.Safire3Pro, 3.6.1.0
-Tecan.At.Instrument.Reader.SunriseMini, 3.6.1.0
-Tecan.At.Instrument.Server, 3.9.1.0
-Tecan.At.Instrument.Stacker.Connect, 3.9.1.0
-Tecan.At.Instrument.Stacker.Server, 3.9.1.0
-Tecan.At.Measurement.BuiltInTest.Common, 3.6.1.0
-Tecan.At.Measurement.Common, 3.6.1.0
-Tecan.At.Measurement.Server, 3.6.1.0
-Tecan.At.XFluor, 2.0.10.0
-Tecan.At.XFluor.Connect.Reader, 2.0.10.0
-Tecan.At.XFluor.Core, 2.0.10.0
-Tecan.At.XFluor.Device, 2.0.10.0
-Tecan.At.XFluor.Device.AMR, 2.0.10.0
-Tecan.At.XFluor.Device.AMRPlus, 2.0.10.0
-Tecan.At.XFluor.Device.GeniosUltra, 2.0.10.0
-Tecan.At.XFluor.Device.Reader, 2.0.10.0
-Tecan.At.XFluor.Device.Safire3, 2.0.10.0
-Tecan.At.XFluor.Device.Safire3Pro, 2.0.10.0
-Tecan.At.XFluor.Device.SunriseMini, 2.0.10.0
-Tecan.At.XFluor.ExcelOutput, 2.0.10.0
-Tecan.At.XFluor.NanoQuant, 2.0.10.0
-Tecan.At.XFluor.ReaderEditor, 2.0.10.0
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{4C4B634E-2D2E-40BE-AFDA-97D9AB9C847F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
-MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
-ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
-LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
-TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dusenbury Crawford, Katharine H</author>
@@ -226,7 +131,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dusenbury Crawford, Katharine H</author>
@@ -320,7 +225,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dusenbury Crawford, Katharine H</author>
@@ -414,7 +319,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dusenbury Crawford, Katharine H</author>
@@ -508,7 +413,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dusenbury Crawford, Katharine H</author>
@@ -602,7 +507,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dusenbury Crawford, Katharine H</author>
@@ -697,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="58">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -871,12 +776,6 @@
   </si>
   <si>
     <t>1/25/2021 11:39:00 AM</t>
-  </si>
-  <si>
-    <t>11:39:37 AM</t>
-  </si>
-  <si>
-    <t>1/25/2021 11:39:46 AM</t>
   </si>
 </sst>
 </file>
@@ -1313,16 +1212,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E714B5-8E76-49A7-9FB0-22ACB6FBDDE3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE957DD-4B1E-4CF1-B789-C10DBCD6B09A}">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1338,7 +1237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1346,7 +1245,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1354,15 +1253,15 @@
         <v>44221</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1370,7 +1269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1378,7 +1277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1386,17 +1285,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1404,7 +1303,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1412,7 +1311,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1423,7 +1322,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1434,20 +1333,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1488,130 +1387,340 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
         <v>-1</v>
       </c>
-      <c r="C24">
-        <v>10</v>
-      </c>
-      <c r="D24">
-        <v>15</v>
-      </c>
-      <c r="E24">
-        <v>5</v>
-      </c>
       <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>-1</v>
+      </c>
+      <c r="I24">
+        <v>17</v>
+      </c>
+      <c r="J24">
+        <v>8</v>
+      </c>
+      <c r="K24">
         <v>1</v>
       </c>
-      <c r="G24">
-        <v>5</v>
-      </c>
-      <c r="H24">
-        <v>8</v>
-      </c>
-      <c r="I24">
+      <c r="L24">
+        <v>11</v>
+      </c>
+      <c r="M24">
         <v>6</v>
       </c>
-      <c r="J24">
-        <v>5</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>4</v>
-      </c>
-      <c r="M24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B25">
-        <v>1336</v>
+        <v>4</v>
       </c>
       <c r="C25">
+        <v>804563</v>
+      </c>
+      <c r="D25">
+        <v>847001</v>
+      </c>
+      <c r="E25">
+        <v>9</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>2291440</v>
+      </c>
+      <c r="H25">
+        <v>2020697</v>
+      </c>
+      <c r="I25">
         <v>8</v>
       </c>
-      <c r="D25">
+      <c r="J25">
+        <v>-2</v>
+      </c>
+      <c r="K25">
         <v>12</v>
       </c>
-      <c r="E25">
-        <v>2901954</v>
-      </c>
-      <c r="F25">
-        <v>2909645</v>
-      </c>
-      <c r="G25">
-        <v>23</v>
-      </c>
-      <c r="H25">
-        <v>5756326</v>
-      </c>
-      <c r="I25">
-        <v>5467299</v>
-      </c>
-      <c r="J25">
-        <v>7</v>
-      </c>
-      <c r="K25">
-        <v>355857</v>
-      </c>
       <c r="L25">
-        <v>339580</v>
+        <v>3</v>
       </c>
       <c r="M25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>399120</v>
       </c>
       <c r="D26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>335364</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>967128</v>
+      </c>
+      <c r="H26">
+        <v>964965</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>7</v>
+      </c>
+      <c r="M26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>178140</v>
+      </c>
+      <c r="D27">
+        <v>217937</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>488929</v>
+      </c>
+      <c r="H27">
+        <v>482451</v>
+      </c>
+      <c r="I27">
+        <v>27</v>
+      </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
+      <c r="K27">
+        <v>10</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>92452</v>
+      </c>
+      <c r="D28">
+        <v>83424</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>12</v>
+      </c>
+      <c r="G28">
+        <v>224252</v>
+      </c>
+      <c r="H28">
+        <v>293340</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <v>6</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>49553</v>
+      </c>
+      <c r="D29">
+        <v>40622</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>-1</v>
+      </c>
+      <c r="G29">
+        <v>103408</v>
+      </c>
+      <c r="H29">
+        <v>146895</v>
+      </c>
+      <c r="I29">
+        <v>-1</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>-2</v>
+      </c>
+      <c r="L29">
+        <v>-2</v>
+      </c>
+      <c r="M29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>30360</v>
+      </c>
+      <c r="D30">
+        <v>28383</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>-1</v>
+      </c>
+      <c r="G30">
+        <v>73513</v>
+      </c>
+      <c r="H30">
+        <v>69376</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>6</v>
+      </c>
+      <c r="L30">
+        <v>-1</v>
+      </c>
+      <c r="M30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>12622</v>
+      </c>
+      <c r="D31">
+        <v>22245</v>
+      </c>
+      <c r="E31">
+        <v>-4</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>63755</v>
+      </c>
+      <c r="H31">
+        <v>43754</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="J31">
+        <v>3</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>7</v>
+      </c>
+      <c r="M31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1621,16 +1730,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE957DD-4B1E-4CF1-B789-C10DBCD6B09A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0FE0C5-4B20-4A31-800C-BDC3CDA40DD1}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1638,7 +1747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1646,7 +1755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1654,7 +1763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1662,15 +1771,15 @@
         <v>44221</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1678,7 +1787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1686,7 +1795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1694,17 +1803,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1712,7 +1821,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1720,7 +1829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1731,7 +1840,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1742,20 +1851,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1796,340 +1905,340 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24">
         <v>6</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
+      <c r="F24">
+        <v>11</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>7</v>
+      </c>
+      <c r="I24">
+        <v>10</v>
+      </c>
+      <c r="J24">
+        <v>10</v>
+      </c>
+      <c r="K24">
         <v>4</v>
       </c>
-      <c r="E24">
+      <c r="L24">
+        <v>5</v>
+      </c>
+      <c r="M24">
         <v>-1</v>
       </c>
-      <c r="F24">
-        <v>3</v>
-      </c>
-      <c r="G24">
-        <v>4</v>
-      </c>
-      <c r="H24">
-        <v>-1</v>
-      </c>
-      <c r="I24">
-        <v>17</v>
-      </c>
-      <c r="J24">
-        <v>8</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>11</v>
-      </c>
-      <c r="M24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B25">
+        <v>1669</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>15</v>
+      </c>
+      <c r="E25">
+        <v>3640446</v>
+      </c>
+      <c r="F25">
+        <v>3659406</v>
+      </c>
+      <c r="G25">
+        <v>25</v>
+      </c>
+      <c r="H25">
+        <v>7313032</v>
+      </c>
+      <c r="I25">
+        <v>7047822</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <v>435272</v>
+      </c>
+      <c r="L25">
+        <v>423752</v>
+      </c>
+      <c r="M25">
         <v>4</v>
       </c>
-      <c r="C25">
-        <v>804563</v>
-      </c>
-      <c r="D25">
-        <v>847001</v>
-      </c>
-      <c r="E25">
-        <v>9</v>
-      </c>
-      <c r="F25">
-        <v>6</v>
-      </c>
-      <c r="G25">
-        <v>2291440</v>
-      </c>
-      <c r="H25">
-        <v>2020697</v>
-      </c>
-      <c r="I25">
-        <v>8</v>
-      </c>
-      <c r="J25">
-        <v>-2</v>
-      </c>
-      <c r="K25">
-        <v>12</v>
-      </c>
-      <c r="L25">
-        <v>3</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
         <v>9</v>
       </c>
-      <c r="C26">
-        <v>399120</v>
-      </c>
-      <c r="D26">
-        <v>335364</v>
-      </c>
       <c r="E26">
-        <v>3</v>
+        <v>1638490</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>1590940</v>
       </c>
       <c r="G26">
-        <v>967128</v>
+        <v>14</v>
       </c>
       <c r="H26">
-        <v>964965</v>
+        <v>3197663</v>
       </c>
       <c r="I26">
-        <v>2</v>
+        <v>3008704</v>
       </c>
       <c r="J26">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="K26">
-        <v>2</v>
+        <v>210358</v>
       </c>
       <c r="L26">
-        <v>7</v>
+        <v>219747</v>
       </c>
       <c r="M26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>864155</v>
+      </c>
+      <c r="F27">
+        <v>810267</v>
+      </c>
+      <c r="G27">
+        <v>84</v>
+      </c>
+      <c r="H27">
+        <v>1436343</v>
+      </c>
+      <c r="I27">
+        <v>1408322</v>
+      </c>
+      <c r="J27">
+        <v>36</v>
+      </c>
+      <c r="K27">
+        <v>104648</v>
+      </c>
+      <c r="L27">
+        <v>129925</v>
+      </c>
+      <c r="M27">
         <v>5</v>
       </c>
-      <c r="C27">
-        <v>178140</v>
-      </c>
-      <c r="D27">
-        <v>217937</v>
-      </c>
-      <c r="E27">
-        <v>5</v>
-      </c>
-      <c r="F27">
-        <v>4</v>
-      </c>
-      <c r="G27">
-        <v>488929</v>
-      </c>
-      <c r="H27">
-        <v>482451</v>
-      </c>
-      <c r="I27">
-        <v>27</v>
-      </c>
-      <c r="J27">
-        <v>5</v>
-      </c>
-      <c r="K27">
-        <v>10</v>
-      </c>
-      <c r="L27">
-        <v>2</v>
-      </c>
-      <c r="M27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>9</v>
+      </c>
+      <c r="E28">
+        <v>385472</v>
+      </c>
+      <c r="F28">
+        <v>382861</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>679514</v>
+      </c>
+      <c r="I28">
+        <v>676590</v>
+      </c>
+      <c r="J28">
         <v>7</v>
       </c>
-      <c r="C28">
-        <v>92452</v>
-      </c>
-      <c r="D28">
-        <v>83424</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>12</v>
-      </c>
-      <c r="G28">
-        <v>224252</v>
-      </c>
-      <c r="H28">
-        <v>293340</v>
-      </c>
-      <c r="I28">
-        <v>5</v>
-      </c>
-      <c r="J28">
+      <c r="K28">
+        <v>54037</v>
+      </c>
+      <c r="L28">
+        <v>56551</v>
+      </c>
+      <c r="M28">
         <v>6</v>
       </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28">
-        <v>4</v>
-      </c>
-      <c r="M28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
         <v>1</v>
       </c>
-      <c r="C29">
-        <v>49553</v>
-      </c>
-      <c r="D29">
-        <v>40622</v>
-      </c>
       <c r="E29">
+        <v>168567</v>
+      </c>
+      <c r="F29">
+        <v>222324</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>337218</v>
+      </c>
+      <c r="I29">
+        <v>338056</v>
+      </c>
+      <c r="J29">
+        <v>6</v>
+      </c>
+      <c r="K29">
+        <v>16851</v>
+      </c>
+      <c r="L29">
+        <v>20993</v>
+      </c>
+      <c r="M29">
         <v>4</v>
       </c>
-      <c r="F29">
-        <v>-1</v>
-      </c>
-      <c r="G29">
-        <v>103408</v>
-      </c>
-      <c r="H29">
-        <v>146895</v>
-      </c>
-      <c r="I29">
-        <v>-1</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>-2</v>
-      </c>
-      <c r="L29">
-        <v>-2</v>
-      </c>
-      <c r="M29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C30">
-        <v>30360</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>28383</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>89895</v>
       </c>
       <c r="F30">
-        <v>-1</v>
+        <v>125786</v>
       </c>
       <c r="G30">
-        <v>73513</v>
+        <v>3</v>
       </c>
       <c r="H30">
-        <v>69376</v>
+        <v>187957</v>
       </c>
       <c r="I30">
-        <v>10</v>
+        <v>179616</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K30">
-        <v>6</v>
+        <v>4632</v>
       </c>
       <c r="L30">
-        <v>-1</v>
+        <v>11823</v>
       </c>
       <c r="M30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C31">
-        <v>12622</v>
+        <v>2</v>
       </c>
       <c r="D31">
-        <v>22245</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>-4</v>
+        <v>62932</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>83233</v>
       </c>
       <c r="G31">
-        <v>63755</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>43754</v>
+        <v>138972</v>
       </c>
       <c r="I31">
-        <v>3</v>
+        <v>141860</v>
       </c>
       <c r="J31">
         <v>3</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>2834</v>
       </c>
       <c r="L31">
-        <v>7</v>
+        <v>17823</v>
       </c>
       <c r="M31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2139,16 +2248,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0FE0C5-4B20-4A31-800C-BDC3CDA40DD1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FD1ECF-0FCF-4686-86B8-8928FDB7A442}">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2156,7 +2265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2164,7 +2273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2172,7 +2281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2180,15 +2289,15 @@
         <v>44221</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2196,7 +2305,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2204,7 +2313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2212,17 +2321,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2230,7 +2339,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2238,7 +2347,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2249,7 +2358,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2260,20 +2369,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -2314,36 +2423,36 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>-4</v>
+      </c>
+      <c r="E24">
+        <v>-2</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <v>8</v>
+      </c>
+      <c r="H24">
         <v>5</v>
       </c>
-      <c r="D24">
-        <v>9</v>
-      </c>
-      <c r="E24">
+      <c r="I24">
         <v>6</v>
       </c>
-      <c r="F24">
-        <v>11</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>7</v>
-      </c>
-      <c r="I24">
-        <v>10</v>
-      </c>
       <c r="J24">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K24">
         <v>4</v>
@@ -2352,302 +2461,302 @@
         <v>5</v>
       </c>
       <c r="M24">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B25">
-        <v>1669</v>
+        <v>1621275</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>1459671</v>
       </c>
       <c r="D25">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E25">
-        <v>3640446</v>
+        <v>64134</v>
       </c>
       <c r="F25">
-        <v>3659406</v>
+        <v>62968</v>
       </c>
       <c r="G25">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="H25">
-        <v>7313032</v>
+        <v>292192</v>
       </c>
       <c r="I25">
-        <v>7047822</v>
+        <v>338237</v>
       </c>
       <c r="J25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K25">
-        <v>435272</v>
+        <v>1662983</v>
       </c>
       <c r="L25">
-        <v>423752</v>
+        <v>1837891</v>
       </c>
       <c r="M25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>850320</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>553226</v>
       </c>
       <c r="D26">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E26">
-        <v>1638490</v>
+        <v>16539</v>
       </c>
       <c r="F26">
-        <v>1590940</v>
+        <v>33533</v>
       </c>
       <c r="G26">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H26">
-        <v>3197663</v>
+        <v>162254</v>
       </c>
       <c r="I26">
-        <v>3008704</v>
+        <v>147502</v>
       </c>
       <c r="J26">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="K26">
-        <v>210358</v>
+        <v>722931</v>
       </c>
       <c r="L26">
-        <v>219747</v>
+        <v>893943</v>
       </c>
       <c r="M26">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B27">
+        <v>415060</v>
+      </c>
+      <c r="C27">
+        <v>316564</v>
+      </c>
+      <c r="D27">
         <v>4</v>
       </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>3</v>
-      </c>
       <c r="E27">
-        <v>864155</v>
+        <v>8150</v>
       </c>
       <c r="F27">
-        <v>810267</v>
+        <v>5680</v>
       </c>
       <c r="G27">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="H27">
-        <v>1436343</v>
+        <v>71580</v>
       </c>
       <c r="I27">
-        <v>1408322</v>
+        <v>61621</v>
       </c>
       <c r="J27">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="K27">
-        <v>104648</v>
+        <v>457262</v>
       </c>
       <c r="L27">
-        <v>129925</v>
+        <v>414742</v>
       </c>
       <c r="M27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>215645</v>
       </c>
       <c r="C28">
+        <v>159192</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>6137</v>
+      </c>
+      <c r="F28">
+        <v>14463</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>45128</v>
+      </c>
+      <c r="I28">
+        <v>43194</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>211361</v>
+      </c>
+      <c r="L28">
+        <v>235140</v>
+      </c>
+      <c r="M28">
         <v>8</v>
       </c>
-      <c r="D28">
-        <v>9</v>
-      </c>
-      <c r="E28">
-        <v>385472</v>
-      </c>
-      <c r="F28">
-        <v>382861</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>679514</v>
-      </c>
-      <c r="I28">
-        <v>676590</v>
-      </c>
-      <c r="J28">
-        <v>7</v>
-      </c>
-      <c r="K28">
-        <v>54037</v>
-      </c>
-      <c r="L28">
-        <v>56551</v>
-      </c>
-      <c r="M28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B29">
+        <v>84261</v>
+      </c>
+      <c r="C29">
+        <v>103085</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>3247</v>
+      </c>
+      <c r="F29">
+        <v>12084</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>9277</v>
+      </c>
+      <c r="I29">
+        <v>19888</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29">
+        <v>96577</v>
+      </c>
+      <c r="L29">
+        <v>112420</v>
+      </c>
+      <c r="M29">
         <v>2</v>
       </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>168567</v>
-      </c>
-      <c r="F29">
-        <v>222324</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>337218</v>
-      </c>
-      <c r="I29">
-        <v>338056</v>
-      </c>
-      <c r="J29">
-        <v>6</v>
-      </c>
-      <c r="K29">
-        <v>16851</v>
-      </c>
-      <c r="L29">
-        <v>20993</v>
-      </c>
-      <c r="M29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B30">
+        <v>72715</v>
+      </c>
+      <c r="C30">
+        <v>62301</v>
+      </c>
+      <c r="D30">
         <v>3</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
       <c r="E30">
-        <v>89895</v>
+        <v>292</v>
       </c>
       <c r="F30">
-        <v>125786</v>
+        <v>3196</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="H30">
-        <v>187957</v>
+        <v>6344</v>
       </c>
       <c r="I30">
-        <v>179616</v>
+        <v>9324</v>
       </c>
       <c r="J30">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K30">
-        <v>4632</v>
+        <v>61856</v>
       </c>
       <c r="L30">
-        <v>11823</v>
+        <v>54536</v>
       </c>
       <c r="M30">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>23198</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>38869</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E31">
-        <v>62932</v>
+        <v>758</v>
       </c>
       <c r="F31">
-        <v>83233</v>
+        <v>198</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H31">
-        <v>138972</v>
+        <v>7022</v>
       </c>
       <c r="I31">
-        <v>141860</v>
+        <v>6799</v>
       </c>
       <c r="J31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K31">
-        <v>2834</v>
+        <v>39038</v>
       </c>
       <c r="L31">
-        <v>17823</v>
+        <v>51613</v>
       </c>
       <c r="M31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2657,16 +2766,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FD1ECF-0FCF-4686-86B8-8928FDB7A442}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9057604-2C4E-4E98-AF9F-A64A93960B03}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
-    </sheetView>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2674,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2682,7 +2789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2690,7 +2797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2698,15 +2805,15 @@
         <v>44221</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2714,7 +2821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2722,7 +2829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2730,17 +2837,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2748,7 +2855,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2756,7 +2863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2767,7 +2874,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2778,20 +2885,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -2832,340 +2939,340 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I24">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K24">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L24">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="M24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B25">
-        <v>1621275</v>
+        <v>3293498</v>
       </c>
       <c r="C25">
-        <v>1459671</v>
+        <v>3648073</v>
       </c>
       <c r="D25">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25">
-        <v>64134</v>
+        <v>5048155</v>
       </c>
       <c r="F25">
-        <v>62968</v>
+        <v>4794377</v>
       </c>
       <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>431205</v>
+      </c>
+      <c r="I25">
+        <v>409466</v>
+      </c>
+      <c r="J25">
         <v>9</v>
       </c>
-      <c r="H25">
-        <v>292192</v>
-      </c>
-      <c r="I25">
-        <v>338237</v>
-      </c>
-      <c r="J25">
+      <c r="K25">
+        <v>4015410</v>
+      </c>
+      <c r="L25">
+        <v>4314482</v>
+      </c>
+      <c r="M25">
         <v>4</v>
       </c>
-      <c r="K25">
-        <v>1662983</v>
-      </c>
-      <c r="L25">
-        <v>1837891</v>
-      </c>
-      <c r="M25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B26">
-        <v>850320</v>
+        <v>2082302</v>
       </c>
       <c r="C26">
-        <v>553226</v>
+        <v>1976333</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E26">
-        <v>16539</v>
+        <v>2209800</v>
       </c>
       <c r="F26">
-        <v>33533</v>
+        <v>2214552</v>
       </c>
       <c r="G26">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H26">
-        <v>162254</v>
+        <v>174102</v>
       </c>
       <c r="I26">
-        <v>147502</v>
+        <v>216021</v>
       </c>
       <c r="J26">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="K26">
-        <v>722931</v>
+        <v>1697735</v>
       </c>
       <c r="L26">
-        <v>893943</v>
+        <v>1831759</v>
       </c>
       <c r="M26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B27">
-        <v>415060</v>
+        <v>1064818</v>
       </c>
       <c r="C27">
-        <v>316564</v>
+        <v>956730</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E27">
-        <v>8150</v>
+        <v>1148826</v>
       </c>
       <c r="F27">
-        <v>5680</v>
+        <v>1024829</v>
       </c>
       <c r="G27">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <v>95860</v>
+      </c>
+      <c r="I27">
+        <v>93888</v>
+      </c>
+      <c r="J27">
+        <v>9</v>
+      </c>
+      <c r="K27">
+        <v>838643</v>
+      </c>
+      <c r="L27">
+        <v>817484</v>
+      </c>
+      <c r="M27">
         <v>2</v>
       </c>
-      <c r="H27">
-        <v>71580</v>
-      </c>
-      <c r="I27">
-        <v>61621</v>
-      </c>
-      <c r="J27">
-        <v>19</v>
-      </c>
-      <c r="K27">
-        <v>457262</v>
-      </c>
-      <c r="L27">
-        <v>414742</v>
-      </c>
-      <c r="M27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B28">
-        <v>215645</v>
+        <v>549842</v>
       </c>
       <c r="C28">
-        <v>159192</v>
+        <v>477471</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28">
-        <v>6137</v>
+        <v>496629</v>
       </c>
       <c r="F28">
-        <v>14463</v>
+        <v>607508</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H28">
-        <v>45128</v>
+        <v>50946</v>
       </c>
       <c r="I28">
-        <v>43194</v>
+        <v>41294</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K28">
-        <v>211361</v>
+        <v>440661</v>
       </c>
       <c r="L28">
-        <v>235140</v>
+        <v>479166</v>
       </c>
       <c r="M28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B29">
-        <v>84261</v>
+        <v>276512</v>
       </c>
       <c r="C29">
-        <v>103085</v>
+        <v>231141</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>3247</v>
+        <v>303847</v>
       </c>
       <c r="F29">
-        <v>12084</v>
+        <v>338408</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>9277</v>
+        <v>14410</v>
       </c>
       <c r="I29">
-        <v>19888</v>
+        <v>32050</v>
       </c>
       <c r="J29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K29">
-        <v>96577</v>
+        <v>238097</v>
       </c>
       <c r="L29">
-        <v>112420</v>
+        <v>242904</v>
       </c>
       <c r="M29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B30">
-        <v>72715</v>
+        <v>147895</v>
       </c>
       <c r="C30">
-        <v>62301</v>
+        <v>131359</v>
       </c>
       <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>152729</v>
+      </c>
+      <c r="F30">
+        <v>109817</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30">
+        <v>18870</v>
+      </c>
+      <c r="I30">
+        <v>15217</v>
+      </c>
+      <c r="J30">
         <v>3</v>
       </c>
-      <c r="E30">
-        <v>292</v>
-      </c>
-      <c r="F30">
-        <v>3196</v>
-      </c>
-      <c r="G30">
-        <v>13</v>
-      </c>
-      <c r="H30">
-        <v>6344</v>
-      </c>
-      <c r="I30">
-        <v>9324</v>
-      </c>
-      <c r="J30">
-        <v>2</v>
-      </c>
       <c r="K30">
-        <v>61856</v>
+        <v>137455</v>
       </c>
       <c r="L30">
-        <v>54536</v>
+        <v>101169</v>
       </c>
       <c r="M30">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B31">
-        <v>23198</v>
+        <v>60683</v>
       </c>
       <c r="C31">
-        <v>38869</v>
+        <v>76084</v>
       </c>
       <c r="D31">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>758</v>
+        <v>88948</v>
       </c>
       <c r="F31">
-        <v>198</v>
+        <v>96177</v>
       </c>
       <c r="G31">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="H31">
-        <v>7022</v>
+        <v>4403</v>
       </c>
       <c r="I31">
-        <v>6799</v>
+        <v>10742</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K31">
-        <v>39038</v>
+        <v>66935</v>
       </c>
       <c r="L31">
-        <v>51613</v>
+        <v>90590</v>
       </c>
       <c r="M31">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3175,14 +3282,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9057604-2C4E-4E98-AF9F-A64A93960B03}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EFB9D7-6E60-4C2D-8098-FCA035AB52BF}">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3190,7 +3297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3198,7 +3305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3206,7 +3313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3214,15 +3321,15 @@
         <v>44221</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3230,7 +3337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3238,7 +3345,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3246,17 +3353,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -3264,7 +3371,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -3272,7 +3379,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -3283,7 +3390,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -3294,20 +3401,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -3348,340 +3455,340 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>-3</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="H24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>-6</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="L24">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B25">
-        <v>3293498</v>
+        <v>2942782</v>
       </c>
       <c r="C25">
-        <v>3648073</v>
+        <v>2588953</v>
       </c>
       <c r="D25">
-        <v>11</v>
+        <v>-1</v>
       </c>
       <c r="E25">
-        <v>5048155</v>
+        <v>1123663</v>
       </c>
       <c r="F25">
-        <v>4794377</v>
+        <v>954722</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H25">
-        <v>431205</v>
+        <v>472663</v>
       </c>
       <c r="I25">
-        <v>409466</v>
+        <v>435249</v>
       </c>
       <c r="J25">
-        <v>9</v>
+        <v>-3</v>
       </c>
       <c r="K25">
-        <v>4015410</v>
+        <v>465951</v>
       </c>
       <c r="L25">
-        <v>4314482</v>
+        <v>473945</v>
       </c>
       <c r="M25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B26">
-        <v>2082302</v>
+        <v>1375626</v>
       </c>
       <c r="C26">
-        <v>1976333</v>
+        <v>1016591</v>
       </c>
       <c r="D26">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E26">
-        <v>2209800</v>
+        <v>536871</v>
       </c>
       <c r="F26">
-        <v>2214552</v>
+        <v>559965</v>
       </c>
       <c r="G26">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H26">
-        <v>174102</v>
+        <v>215862</v>
       </c>
       <c r="I26">
-        <v>216021</v>
+        <v>211406</v>
       </c>
       <c r="J26">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K26">
-        <v>1697735</v>
+        <v>248876</v>
       </c>
       <c r="L26">
-        <v>1831759</v>
+        <v>235268</v>
       </c>
       <c r="M26">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B27">
-        <v>1064818</v>
+        <v>757047</v>
       </c>
       <c r="C27">
-        <v>956730</v>
+        <v>615331</v>
       </c>
       <c r="D27">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>1148826</v>
+        <v>284545</v>
       </c>
       <c r="F27">
-        <v>1024829</v>
+        <v>282980</v>
       </c>
       <c r="G27">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="H27">
-        <v>95860</v>
+        <v>127259</v>
       </c>
       <c r="I27">
-        <v>93888</v>
+        <v>103277</v>
       </c>
       <c r="J27">
-        <v>9</v>
+        <v>-2</v>
       </c>
       <c r="K27">
-        <v>838643</v>
+        <v>102315</v>
       </c>
       <c r="L27">
-        <v>817484</v>
+        <v>97570</v>
       </c>
       <c r="M27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B28">
-        <v>549842</v>
+        <v>339679</v>
       </c>
       <c r="C28">
-        <v>477471</v>
+        <v>295432</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E28">
-        <v>496629</v>
+        <v>150649</v>
       </c>
       <c r="F28">
-        <v>607508</v>
+        <v>135728</v>
       </c>
       <c r="G28">
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="H28">
-        <v>50946</v>
+        <v>39127</v>
       </c>
       <c r="I28">
-        <v>41294</v>
+        <v>70470</v>
       </c>
       <c r="J28">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K28">
-        <v>440661</v>
+        <v>72824</v>
       </c>
       <c r="L28">
-        <v>479166</v>
+        <v>43031</v>
       </c>
       <c r="M28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B29">
-        <v>276512</v>
+        <v>200576</v>
       </c>
       <c r="C29">
-        <v>231141</v>
+        <v>143854</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>-7</v>
       </c>
       <c r="E29">
-        <v>303847</v>
+        <v>65482</v>
       </c>
       <c r="F29">
-        <v>338408</v>
+        <v>78607</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H29">
-        <v>14410</v>
+        <v>20974</v>
       </c>
       <c r="I29">
-        <v>32050</v>
+        <v>18878</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29">
-        <v>238097</v>
+        <v>10087</v>
       </c>
       <c r="L29">
-        <v>242904</v>
+        <v>19865</v>
       </c>
       <c r="M29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B30">
-        <v>147895</v>
+        <v>87095</v>
       </c>
       <c r="C30">
-        <v>131359</v>
+        <v>62764</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>-7</v>
       </c>
       <c r="E30">
-        <v>152729</v>
+        <v>26603</v>
       </c>
       <c r="F30">
-        <v>109817</v>
+        <v>34206</v>
       </c>
       <c r="G30">
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="H30">
-        <v>18870</v>
+        <v>6221</v>
       </c>
       <c r="I30">
-        <v>15217</v>
+        <v>12742</v>
       </c>
       <c r="J30">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="K30">
-        <v>137455</v>
+        <v>17243</v>
       </c>
       <c r="L30">
-        <v>101169</v>
+        <v>6293</v>
       </c>
       <c r="M30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B31">
-        <v>60683</v>
+        <v>55187</v>
       </c>
       <c r="C31">
-        <v>76084</v>
+        <v>27903</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E31">
-        <v>88948</v>
+        <v>14915</v>
       </c>
       <c r="F31">
-        <v>96177</v>
+        <v>26129</v>
       </c>
       <c r="G31">
-        <v>-1</v>
+        <v>-6</v>
       </c>
       <c r="H31">
-        <v>4403</v>
+        <v>8033</v>
       </c>
       <c r="I31">
-        <v>10742</v>
+        <v>13368</v>
       </c>
       <c r="J31">
-        <v>9</v>
+        <v>-3</v>
       </c>
       <c r="K31">
-        <v>66935</v>
+        <v>10856</v>
       </c>
       <c r="L31">
-        <v>90590</v>
+        <v>8250</v>
       </c>
       <c r="M31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3691,522 +3798,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EFB9D7-6E60-4C2D-8098-FCA035AB52BF}">
-  <dimension ref="A1:M36"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18">
-        <v>1000</v>
-      </c>
-      <c r="F18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3">
-        <v>2</v>
-      </c>
-      <c r="D23" s="3">
-        <v>3</v>
-      </c>
-      <c r="E23" s="3">
-        <v>4</v>
-      </c>
-      <c r="F23" s="3">
-        <v>5</v>
-      </c>
-      <c r="G23" s="3">
-        <v>6</v>
-      </c>
-      <c r="H23" s="3">
-        <v>7</v>
-      </c>
-      <c r="I23" s="3">
-        <v>8</v>
-      </c>
-      <c r="J23" s="3">
-        <v>9</v>
-      </c>
-      <c r="K23" s="3">
-        <v>10</v>
-      </c>
-      <c r="L23" s="3">
-        <v>11</v>
-      </c>
-      <c r="M23" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24">
-        <v>-3</v>
-      </c>
-      <c r="C24">
-        <v>-1</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>-3</v>
-      </c>
-      <c r="G24">
-        <v>-3</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>-6</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>-7</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25">
-        <v>2942782</v>
-      </c>
-      <c r="C25">
-        <v>2588953</v>
-      </c>
-      <c r="D25">
-        <v>-1</v>
-      </c>
-      <c r="E25">
-        <v>1123663</v>
-      </c>
-      <c r="F25">
-        <v>954722</v>
-      </c>
-      <c r="G25">
-        <v>7</v>
-      </c>
-      <c r="H25">
-        <v>472663</v>
-      </c>
-      <c r="I25">
-        <v>435249</v>
-      </c>
-      <c r="J25">
-        <v>-3</v>
-      </c>
-      <c r="K25">
-        <v>465951</v>
-      </c>
-      <c r="L25">
-        <v>473945</v>
-      </c>
-      <c r="M25">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26">
-        <v>1375626</v>
-      </c>
-      <c r="C26">
-        <v>1016591</v>
-      </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-      <c r="E26">
-        <v>536871</v>
-      </c>
-      <c r="F26">
-        <v>559965</v>
-      </c>
-      <c r="G26">
-        <v>12</v>
-      </c>
-      <c r="H26">
-        <v>215862</v>
-      </c>
-      <c r="I26">
-        <v>211406</v>
-      </c>
-      <c r="J26">
-        <v>12</v>
-      </c>
-      <c r="K26">
-        <v>248876</v>
-      </c>
-      <c r="L26">
-        <v>235268</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27">
-        <v>757047</v>
-      </c>
-      <c r="C27">
-        <v>615331</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>284545</v>
-      </c>
-      <c r="F27">
-        <v>282980</v>
-      </c>
-      <c r="G27">
-        <v>24</v>
-      </c>
-      <c r="H27">
-        <v>127259</v>
-      </c>
-      <c r="I27">
-        <v>103277</v>
-      </c>
-      <c r="J27">
-        <v>-2</v>
-      </c>
-      <c r="K27">
-        <v>102315</v>
-      </c>
-      <c r="L27">
-        <v>97570</v>
-      </c>
-      <c r="M27">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28">
-        <v>339679</v>
-      </c>
-      <c r="C28">
-        <v>295432</v>
-      </c>
-      <c r="D28">
-        <v>6</v>
-      </c>
-      <c r="E28">
-        <v>150649</v>
-      </c>
-      <c r="F28">
-        <v>135728</v>
-      </c>
-      <c r="G28">
-        <v>-3</v>
-      </c>
-      <c r="H28">
-        <v>39127</v>
-      </c>
-      <c r="I28">
-        <v>70470</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>72824</v>
-      </c>
-      <c r="L28">
-        <v>43031</v>
-      </c>
-      <c r="M28">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29">
-        <v>200576</v>
-      </c>
-      <c r="C29">
-        <v>143854</v>
-      </c>
-      <c r="D29">
-        <v>-7</v>
-      </c>
-      <c r="E29">
-        <v>65482</v>
-      </c>
-      <c r="F29">
-        <v>78607</v>
-      </c>
-      <c r="G29">
-        <v>-2</v>
-      </c>
-      <c r="H29">
-        <v>20974</v>
-      </c>
-      <c r="I29">
-        <v>18878</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>10087</v>
-      </c>
-      <c r="L29">
-        <v>19865</v>
-      </c>
-      <c r="M29">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30">
-        <v>87095</v>
-      </c>
-      <c r="C30">
-        <v>62764</v>
-      </c>
-      <c r="D30">
-        <v>-7</v>
-      </c>
-      <c r="E30">
-        <v>26603</v>
-      </c>
-      <c r="F30">
-        <v>34206</v>
-      </c>
-      <c r="G30">
-        <v>-3</v>
-      </c>
-      <c r="H30">
-        <v>6221</v>
-      </c>
-      <c r="I30">
-        <v>12742</v>
-      </c>
-      <c r="J30">
-        <v>-1</v>
-      </c>
-      <c r="K30">
-        <v>17243</v>
-      </c>
-      <c r="L30">
-        <v>6293</v>
-      </c>
-      <c r="M30">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31">
-        <v>55187</v>
-      </c>
-      <c r="C31">
-        <v>27903</v>
-      </c>
-      <c r="D31">
-        <v>5</v>
-      </c>
-      <c r="E31">
-        <v>14915</v>
-      </c>
-      <c r="F31">
-        <v>26129</v>
-      </c>
-      <c r="G31">
-        <v>-6</v>
-      </c>
-      <c r="H31">
-        <v>8033</v>
-      </c>
-      <c r="I31">
-        <v>13368</v>
-      </c>
-      <c r="J31">
-        <v>-3</v>
-      </c>
-      <c r="K31">
-        <v>10856</v>
-      </c>
-      <c r="L31">
-        <v>8250</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FE5241-38BE-4DAB-B42C-1399CFD01C4D}">
   <dimension ref="A1:M36"/>
   <sheetViews>
@@ -4214,9 +3805,9 @@
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4224,7 +3815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4232,7 +3823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4240,7 +3831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -4248,7 +3839,7 @@
         <v>44221</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4256,7 +3847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -4264,7 +3855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -4272,7 +3863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4280,17 +3871,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -4298,7 +3889,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -4306,7 +3897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -4317,7 +3908,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -4328,7 +3919,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -4336,12 +3927,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -4382,7 +3973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -4423,7 +4014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
@@ -4464,7 +4055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
@@ -4505,7 +4096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
@@ -4546,7 +4137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
@@ -4587,7 +4178,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
@@ -4628,7 +4219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>34</v>
       </c>
@@ -4669,7 +4260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
@@ -4710,7 +4301,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>

</xml_diff>